<commit_message>
export with translate and formatting
</commit_message>
<xml_diff>
--- a/Code/public/Venator_Consuting_Exported_file_posting_1_1.xlsx
+++ b/Code/public/Venator_Consuting_Exported_file_posting_1_1.xlsx
@@ -385,323 +385,262 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="4" width="10" customWidth="1"/>
+    <col min="1" max="2" width="10" customWidth="1"/>
+    <col min="3" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="9" width="25" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="12" width="25" customWidth="1"/>
-    <col min="14" max="28" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="15" width="25" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="22" width="25" customWidth="1"/>
+    <col min="23" max="23" width="10" customWidth="1"/>
+    <col min="24" max="69" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
-        <v>Id</v>
+        <v>Mandant</v>
       </c>
       <c r="B1" t="str">
-        <v>procedureId</v>
+        <v>Buchungskreis</v>
       </c>
       <c r="C1" t="str">
-        <v>client</v>
+        <v>Belegnummer</v>
       </c>
       <c r="D1" t="str">
-        <v>companyCode</v>
+        <v>Belegdatum</v>
       </c>
       <c r="E1" t="str">
-        <v>recordNumber</v>
+        <v>Kontotyp</v>
       </c>
       <c r="F1" t="str">
-        <v>documentNumber</v>
+        <v>Gegenkontotyp</v>
       </c>
       <c r="G1" t="str">
-        <v>documentNumber2</v>
+        <v>Kontonummer</v>
       </c>
       <c r="H1" t="str">
-        <v>assignment</v>
+        <v>Kontobezeichnung</v>
       </c>
       <c r="I1" t="str">
-        <v>reference</v>
+        <v>Kontonummer Gegenkonto</v>
       </c>
       <c r="J1" t="str">
-        <v>documentTypeNumber</v>
+        <v>Bezeichnung Kreditorenkonto</v>
       </c>
       <c r="K1" t="str">
-        <v>documentTypeName</v>
+        <v>Saldo EUR</v>
       </c>
       <c r="L1" t="str">
-        <v>documentTypeNew</v>
+        <v>Umsatz Soll EUR</v>
       </c>
       <c r="M1" t="str">
-        <v>documentDate</v>
+        <v>Umsatz Haben EUR</v>
       </c>
       <c r="N1" t="str">
-        <v>postingDate</v>
+        <v>Stapelnummer</v>
       </c>
       <c r="O1" t="str">
-        <v>dueDate</v>
+        <v>Buchungssatznummer</v>
       </c>
       <c r="P1" t="str">
-        <v>dueDateNew</v>
+        <v>Geschäftsjahr</v>
       </c>
       <c r="Q1" t="str">
-        <v>fiscalYear</v>
+        <v>Steuerbetrag</v>
       </c>
       <c r="R1" t="str">
-        <v>postingPeriod</v>
+        <v>Leistungsdatum</v>
       </c>
       <c r="S1" t="str">
-        <v>executionDate</v>
+        <v>Fälligkeitsdatum</v>
       </c>
       <c r="T1" t="str">
-        <v>accountType</v>
+        <v>ID des Rechnungslegungsbereichs</v>
       </c>
       <c r="U1" t="str">
-        <v>accountNumber</v>
+        <v>Zuordnung</v>
       </c>
       <c r="V1" t="str">
-        <v>accountName</v>
+        <v>Referenz</v>
       </c>
       <c r="W1" t="str">
-        <v>GLAccountNumber</v>
+        <v>Belegart</v>
       </c>
       <c r="X1" t="str">
-        <v>GLAccountName</v>
+        <v>Buchungsdatum</v>
       </c>
       <c r="Y1" t="str">
-        <v>debtorNumber</v>
+        <v>Hauptbuchkonto</v>
       </c>
       <c r="Z1" t="str">
-        <v>debtorName</v>
+        <v>Debitorenkonto</v>
       </c>
       <c r="AA1" t="str">
-        <v>creditorNumber</v>
+        <v>Bezeichnung Debitorenkonto</v>
       </c>
       <c r="AB1" t="str">
-        <v>creditorName</v>
+        <v>Kreditorenkonto</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>Bezeichnung Kreditorenkonto</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>Sachkonto Gegenkonto</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>Bezeichnung Gegenkonto Sachkonto</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>Debitorenkonto Gegenkonto</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>Bezeichnung Gegenkonto Debitor</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>Kreditorenkonto Gegenkonto</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>Bezeichnung Gegenkonto Kreditor</v>
+      </c>
+      <c r="AJ1" t="str">
+        <v>Soll / Haben</v>
+      </c>
+      <c r="AK1" t="str">
+        <v>Saldo Belegwährung</v>
+      </c>
+      <c r="AL1" t="str">
+        <v>Belegfeld 2</v>
+      </c>
+      <c r="AM1" t="str">
+        <v>Umrechnungskurs</v>
+      </c>
+      <c r="AN1" t="str">
+        <v>Belegwährung</v>
+      </c>
+      <c r="AO1" t="str">
+        <v>Kostenstelle 1</v>
+      </c>
+      <c r="AP1" t="str">
+        <v>Kostenstelle 2</v>
+      </c>
+      <c r="AQ1" t="str">
+        <v>Umsatzsteuerschlüssel</v>
+      </c>
+      <c r="AR1" t="str">
+        <v>Buchungstext</v>
+      </c>
+      <c r="AS1" t="str">
+        <v>Steuersatz</v>
+      </c>
+      <c r="AT1" t="str">
+        <v>EU Steuersatz</v>
+      </c>
+      <c r="AU1" t="str">
+        <v>Kennung EB-Buchung</v>
+      </c>
+      <c r="AV1" t="str">
+        <v>Buchungsperiode</v>
+      </c>
+      <c r="AW1" t="str">
+        <v>Beleglink</v>
+      </c>
+      <c r="AX1" t="str">
+        <v>Skonto EUR</v>
+      </c>
+      <c r="AY1" t="str">
+        <v>Belegkopftext</v>
+      </c>
+      <c r="AZ1" t="str">
+        <v>Buchungsschlüssel</v>
+      </c>
+      <c r="BA1" t="str">
+        <v>Steuerbetrag Soll</v>
+      </c>
+      <c r="BB1" t="str">
+        <v>Steuerbetrag Haben</v>
+      </c>
+      <c r="BC1" t="str">
+        <v>Ausgleichsbeleg</v>
+      </c>
+      <c r="BD1" t="str">
+        <v>Datum des Ausgleichs</v>
+      </c>
+      <c r="BE1" t="str">
+        <v>Generalumkehr (GU)</v>
+      </c>
+      <c r="BF1" t="str">
+        <v>Art der Beleginformation 1</v>
+      </c>
+      <c r="BG1" t="str">
+        <v>Inhalt der Beleginformation 1</v>
+      </c>
+      <c r="BH1" t="str">
+        <v>Art der Beleginformation 2</v>
+      </c>
+      <c r="BI1" t="str">
+        <v>Inhalt der Beleginformation 2</v>
+      </c>
+      <c r="BJ1" t="str">
+        <v>Art der Beleginformation 3</v>
+      </c>
+      <c r="BK1" t="str">
+        <v>Inhalt der Beleginformation 3</v>
+      </c>
+      <c r="BL1" t="str">
+        <v>Art der Beleginformation 4</v>
+      </c>
+      <c r="BM1" t="str">
+        <v>Inhalt der Beleginformation 4</v>
+      </c>
+      <c r="BN1" t="str">
+        <v>Art der Beleginformation 5</v>
+      </c>
+      <c r="BO1" t="str">
+        <v>Inhalt der Beleginformation 5</v>
+      </c>
+      <c r="BP1" t="str">
+        <v>Art der Beleginformation 6</v>
+      </c>
+      <c r="BQ1" t="str">
+        <v>Inhalt der Beleginformation 6</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5049</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="str">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>43615.875</v>
+      </c>
+      <c r="E2" t="str">
+        <v>K</v>
+      </c>
+      <c r="G2" t="str">
+        <v>970</v>
+      </c>
+      <c r="K2" t="str">
+        <v>-4270.00</v>
+      </c>
+      <c r="L2" t="str">
+        <v>0.00</v>
+      </c>
+      <c r="M2" t="str">
+        <v>4270.00</v>
+      </c>
+      <c r="S2" s="1">
+        <v>43828.91666666667</v>
+      </c>
+      <c r="V2" t="str">
         <v>0</v>
       </c>
-      <c r="M2" s="1">
-        <v>43585.875</v>
-      </c>
-      <c r="O2" s="1">
-        <v>43737.875</v>
-      </c>
-      <c r="T2" t="str">
-        <v>K</v>
-      </c>
-      <c r="U2" t="str">
-        <v>27</v>
-      </c>
-      <c r="V2" t="str">
-        <v>ff</v>
-      </c>
-      <c r="AA2" t="str">
+      <c r="W2" t="str">
+        <v>ZP</v>
+      </c>
+      <c r="AB2" t="str">
         <v>1200</v>
       </c>
-      <c r="AB2" t="str">
+      <c r="AC2" t="str">
         <v>ffff</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5050</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="str">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>43591.875</v>
-      </c>
-      <c r="O3" s="1">
-        <v>43737.875</v>
-      </c>
-      <c r="T3" t="str">
-        <v>K</v>
-      </c>
-      <c r="U3" t="str">
-        <v>27</v>
-      </c>
-      <c r="V3" t="str">
-        <v>ff</v>
-      </c>
-      <c r="AA3" t="str">
-        <v>1200</v>
-      </c>
-      <c r="AB3" t="str">
-        <v>ffff</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5051</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="I4" t="str">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1">
-        <v>43591.875</v>
-      </c>
-      <c r="O4" s="1">
-        <v>43737.875</v>
-      </c>
-      <c r="T4" t="str">
-        <v>K</v>
-      </c>
-      <c r="U4" t="str">
-        <v>27</v>
-      </c>
-      <c r="V4" t="str">
-        <v>ff</v>
-      </c>
-      <c r="AA4" t="str">
-        <v>1200</v>
-      </c>
-      <c r="AB4" t="str">
-        <v>ffff</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5052</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="str">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1">
-        <v>43607.875</v>
-      </c>
-      <c r="O5" s="1">
-        <v>43737.875</v>
-      </c>
-      <c r="T5" t="str">
-        <v>K</v>
-      </c>
-      <c r="U5" t="str">
-        <v>27</v>
-      </c>
-      <c r="V5" t="str">
-        <v>ff</v>
-      </c>
-      <c r="AA5" t="str">
-        <v>1200</v>
-      </c>
-      <c r="AB5" t="str">
-        <v>ffff</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5053</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="I6" t="str">
-        <v>0</v>
-      </c>
-      <c r="M6" s="1">
-        <v>43669.875</v>
-      </c>
-      <c r="O6" s="1">
-        <v>43737.875</v>
-      </c>
-      <c r="T6" t="str">
-        <v>K</v>
-      </c>
-      <c r="U6" t="str">
-        <v>27</v>
-      </c>
-      <c r="V6" t="str">
-        <v>ff</v>
-      </c>
-      <c r="AA6" t="str">
-        <v>1200</v>
-      </c>
-      <c r="AB6" t="str">
-        <v>ffff</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5054</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="I7" t="str">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1">
-        <v>43737.875</v>
-      </c>
-      <c r="O7" s="1">
-        <v>43737.875</v>
-      </c>
-      <c r="T7" t="str">
-        <v>K</v>
-      </c>
-      <c r="U7" t="str">
-        <v>27</v>
-      </c>
-      <c r="V7" t="str">
-        <v>ff</v>
-      </c>
-      <c r="AA7" t="str">
-        <v>1200</v>
-      </c>
-      <c r="AB7" t="str">
-        <v>ffff</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5055</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="I8" t="str">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1">
-        <v>43737.875</v>
-      </c>
-      <c r="O8" s="1">
-        <v>43737.875</v>
-      </c>
-      <c r="T8" t="str">
-        <v>K</v>
-      </c>
-      <c r="U8" t="str">
-        <v>27</v>
-      </c>
-      <c r="V8" t="str">
-        <v>ff</v>
-      </c>
-      <c r="AA8" t="str">
-        <v>1200</v>
-      </c>
-      <c r="AB8" t="str">
-        <v>ffff</v>
+      <c r="AR2" t="str">
+        <v>RE Landgard 05/2019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>